<commit_message>
actualización al 9/04/2020 T 3
</commit_message>
<xml_diff>
--- a/dolartoday.xlsx
+++ b/dolartoday.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3417" uniqueCount="3415">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3418" uniqueCount="3416">
   <si>
     <t>Cotizaciones corresponden al CIERRE del dia</t>
   </si>
@@ -10259,6 +10259,9 @@
   </si>
   <si>
     <t>4-7-2020</t>
+  </si>
+  <si>
+    <t>4-8-2020</t>
   </si>
 </sst>
 </file>
@@ -10395,122 +10398,122 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>DolarToday!$A$3381:$A$3411</c:f>
+              <c:f>DolarToday!$A$3382:$A$3412</c:f>
               <c:strCache>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>3-8-2020</c:v>
+                  <c:v>3-9-2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3-9-2020</c:v>
+                  <c:v>3-10-2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3-10-2020</c:v>
+                  <c:v>3-11-2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3-11-2020</c:v>
+                  <c:v>3-12-2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3-12-2020</c:v>
+                  <c:v>3-13-2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3-13-2020</c:v>
+                  <c:v>3-14-2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3-14-2020</c:v>
+                  <c:v>3-15-2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3-15-2020</c:v>
+                  <c:v>3-16-2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3-16-2020</c:v>
+                  <c:v>3-17-2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3-17-2020</c:v>
+                  <c:v>3-18-2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3-18-2020</c:v>
+                  <c:v>3-19-2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3-19-2020</c:v>
+                  <c:v>3-20-2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3-20-2020</c:v>
+                  <c:v>3-21-2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3-21-2020</c:v>
+                  <c:v>3-22-2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3-22-2020</c:v>
+                  <c:v>3-23-2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3-23-2020</c:v>
+                  <c:v>3-24-2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3-24-2020</c:v>
+                  <c:v>3-25-2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3-25-2020</c:v>
+                  <c:v>3-26-2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3-26-2020</c:v>
+                  <c:v>3-27-2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3-27-2020</c:v>
+                  <c:v>3-28-2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3-28-2020</c:v>
+                  <c:v>3-29-2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>3-29-2020</c:v>
+                  <c:v>3-30-2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>3-30-2020</c:v>
+                  <c:v>3-31-2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3-31-2020</c:v>
+                  <c:v>4-1-2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4-1-2020</c:v>
+                  <c:v>4-2-2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4-2-2020</c:v>
+                  <c:v>4-3-2020</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4-3-2020</c:v>
+                  <c:v>4-4-2020</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4-4-2020</c:v>
+                  <c:v>4-5-2020</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4-5-2020</c:v>
+                  <c:v>4-6-2020</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4-6-2020</c:v>
+                  <c:v>4-7-2020</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4-7-2020</c:v>
+                  <c:v>4-8-2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DolarToday!$B$3381:$B$3411</c:f>
+              <c:f>DolarToday!$B$3382:$B$3412</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>76232.75</c:v>
+                  <c:v>76103.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>76103.62</c:v>
+                  <c:v>76403.82</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>76403.82</c:v>
+                  <c:v>82340.22</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>82340.22</c:v>
+                  <c:v>80023.18</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>80023.18</c:v>
@@ -10522,25 +10525,25 @@
                   <c:v>80023.18</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>80023.18</c:v>
+                  <c:v>76713.38</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>76713.38</c:v>
+                  <c:v>75724.82</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>75724.82</c:v>
+                  <c:v>72731.72</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>72731.72</c:v>
+                  <c:v>71842.92</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>71842.92</c:v>
+                  <c:v>72931.65</c:v>
                 </c:pt>
                 <c:pt idx="12">
                   <c:v>72931.65</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>72931.65</c:v>
+                  <c:v>75184.82</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>75184.82</c:v>
@@ -10552,7 +10555,7 @@
                   <c:v>75184.82</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>75184.82</c:v>
+                  <c:v>84723.01</c:v>
                 </c:pt>
                 <c:pt idx="18">
                   <c:v>84723.01</c:v>
@@ -10561,19 +10564,19 @@
                   <c:v>84723.01</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>84723.01</c:v>
+                  <c:v>84581.04</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>84581.04</c:v>
+                  <c:v>87076.65</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>87076.65</c:v>
+                  <c:v>87396.82</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>87396.82</c:v>
+                  <c:v>89168.7</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>89168.7</c:v>
+                  <c:v>94120.28</c:v>
                 </c:pt>
                 <c:pt idx="25">
                   <c:v>94120.28</c:v>
@@ -10582,13 +10585,13 @@
                   <c:v>94120.28</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>94120.28</c:v>
+                  <c:v>99043.72</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>99043.72</c:v>
+                  <c:v>105729.27</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>105729.27</c:v>
+                  <c:v>117395.02</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>117395.02</c:v>
@@ -10998,7 +11001,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3411"/>
+  <dimension ref="A1:K3412"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -38306,16 +38309,6 @@
       <c r="B3409">
         <v>99043.72</v>
       </c>
-      <c r="D3409" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3409" s="3"/>
-      <c r="F3409" s="3"/>
-      <c r="G3409" s="3"/>
-      <c r="H3409" s="3"/>
-      <c r="I3409" s="3"/>
-      <c r="J3409" s="3"/>
-      <c r="K3409" s="3"/>
     </row>
     <row r="3410" spans="1:11">
       <c r="A3410" t="s">
@@ -38324,16 +38317,16 @@
       <c r="B3410">
         <v>105729.27</v>
       </c>
-      <c r="D3410" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3410" s="4"/>
-      <c r="F3410" s="4"/>
-      <c r="G3410" s="4"/>
-      <c r="H3410" s="4"/>
-      <c r="I3410" s="4"/>
-      <c r="J3410" s="4"/>
-      <c r="K3410" s="4"/>
+      <c r="D3410" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3410" s="3"/>
+      <c r="F3410" s="3"/>
+      <c r="G3410" s="3"/>
+      <c r="H3410" s="3"/>
+      <c r="I3410" s="3"/>
+      <c r="J3410" s="3"/>
+      <c r="K3410" s="3"/>
     </row>
     <row r="3411" spans="1:11">
       <c r="A3411" t="s">
@@ -38342,7 +38335,9 @@
       <c r="B3411">
         <v>117395.02</v>
       </c>
-      <c r="D3411" s="4"/>
+      <c r="D3411" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E3411" s="4"/>
       <c r="F3411" s="4"/>
       <c r="G3411" s="4"/>
@@ -38351,12 +38346,28 @@
       <c r="J3411" s="4"/>
       <c r="K3411" s="4"/>
     </row>
+    <row r="3412" spans="1:11">
+      <c r="A3412" t="s">
+        <v>3415</v>
+      </c>
+      <c r="B3412">
+        <v>117395.02</v>
+      </c>
+      <c r="D3412" s="4"/>
+      <c r="E3412" s="4"/>
+      <c r="F3412" s="4"/>
+      <c r="G3412" s="4"/>
+      <c r="H3412" s="4"/>
+      <c r="I3412" s="4"/>
+      <c r="J3412" s="4"/>
+      <c r="K3412" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D19:K19"/>
     <mergeCell ref="D20:K21"/>
-    <mergeCell ref="D3409:K3409"/>
-    <mergeCell ref="D3410:K3411"/>
+    <mergeCell ref="D3410:K3410"/>
+    <mergeCell ref="D3411:K3412"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Súper Actualización de componentes y Datos
</commit_message>
<xml_diff>
--- a/dolartoday.xlsx
+++ b/dolartoday.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3421" uniqueCount="3419">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3422" uniqueCount="3420">
   <si>
     <t>Cotizaciones corresponden al CIERRE del dia</t>
   </si>
@@ -10271,6 +10271,9 @@
   </si>
   <si>
     <t>4-11-2020</t>
+  </si>
+  <si>
+    <t>4-12-2020</t>
   </si>
 </sst>
 </file>
@@ -10407,108 +10410,108 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>DolarToday!$A$3385:$A$3415</c:f>
+              <c:f>DolarToday!$A$3386:$A$3416</c:f>
               <c:strCache>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>3-12-2020</c:v>
+                  <c:v>3-13-2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>3-13-2020</c:v>
+                  <c:v>3-14-2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3-14-2020</c:v>
+                  <c:v>3-15-2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3-15-2020</c:v>
+                  <c:v>3-16-2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3-16-2020</c:v>
+                  <c:v>3-17-2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3-17-2020</c:v>
+                  <c:v>3-18-2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3-18-2020</c:v>
+                  <c:v>3-19-2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3-19-2020</c:v>
+                  <c:v>3-20-2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3-20-2020</c:v>
+                  <c:v>3-21-2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3-21-2020</c:v>
+                  <c:v>3-22-2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3-22-2020</c:v>
+                  <c:v>3-23-2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3-23-2020</c:v>
+                  <c:v>3-24-2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3-24-2020</c:v>
+                  <c:v>3-25-2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3-25-2020</c:v>
+                  <c:v>3-26-2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3-26-2020</c:v>
+                  <c:v>3-27-2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>3-27-2020</c:v>
+                  <c:v>3-28-2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3-28-2020</c:v>
+                  <c:v>3-29-2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>3-29-2020</c:v>
+                  <c:v>3-30-2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3-30-2020</c:v>
+                  <c:v>3-31-2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>3-31-2020</c:v>
+                  <c:v>4-1-2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4-1-2020</c:v>
+                  <c:v>4-2-2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>4-2-2020</c:v>
+                  <c:v>4-3-2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4-3-2020</c:v>
+                  <c:v>4-4-2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>4-4-2020</c:v>
+                  <c:v>4-5-2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>4-5-2020</c:v>
+                  <c:v>4-6-2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4-6-2020</c:v>
+                  <c:v>4-7-2020</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>4-7-2020</c:v>
+                  <c:v>4-8-2020</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4-8-2020</c:v>
+                  <c:v>4-9-2020</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>4-9-2020</c:v>
+                  <c:v>4-10-2020</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>4-10-2020</c:v>
+                  <c:v>4-11-2020</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4-11-2020</c:v>
+                  <c:v>4-12-2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DolarToday!$B$3385:$B$3415</c:f>
+              <c:f>DolarToday!$B$3386:$B$3416</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
@@ -10522,25 +10525,25 @@
                   <c:v>80023.18</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>80023.18</c:v>
+                  <c:v>76713.38</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>76713.38</c:v>
+                  <c:v>75724.82</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>75724.82</c:v>
+                  <c:v>72731.72</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>72731.72</c:v>
+                  <c:v>71842.92</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>71842.92</c:v>
+                  <c:v>72931.65</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>72931.65</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>72931.65</c:v>
+                  <c:v>75184.82</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>75184.82</c:v>
@@ -10552,7 +10555,7 @@
                   <c:v>75184.82</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>75184.82</c:v>
+                  <c:v>84723.01</c:v>
                 </c:pt>
                 <c:pt idx="14">
                   <c:v>84723.01</c:v>
@@ -10561,19 +10564,19 @@
                   <c:v>84723.01</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>84723.01</c:v>
+                  <c:v>84581.04</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>84581.04</c:v>
+                  <c:v>87076.65</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>87076.65</c:v>
+                  <c:v>87396.82</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>87396.82</c:v>
+                  <c:v>89168.7</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>89168.7</c:v>
+                  <c:v>94120.28</c:v>
                 </c:pt>
                 <c:pt idx="21">
                   <c:v>94120.28</c:v>
@@ -10582,13 +10585,13 @@
                   <c:v>94120.28</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>94120.28</c:v>
+                  <c:v>99043.72</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>99043.72</c:v>
+                  <c:v>105729.27</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>105729.27</c:v>
+                  <c:v>117395.02</c:v>
                 </c:pt>
                 <c:pt idx="26">
                   <c:v>117395.02</c:v>
@@ -10603,7 +10606,7 @@
                   <c:v>117395.02</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>117395.02</c:v>
+                  <c:v>135833.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11010,7 +11013,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3415"/>
+  <dimension ref="A1:K3416"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -38350,16 +38353,6 @@
       <c r="B3413">
         <v>117395.02</v>
       </c>
-      <c r="D3413" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3413" s="3"/>
-      <c r="F3413" s="3"/>
-      <c r="G3413" s="3"/>
-      <c r="H3413" s="3"/>
-      <c r="I3413" s="3"/>
-      <c r="J3413" s="3"/>
-      <c r="K3413" s="3"/>
     </row>
     <row r="3414" spans="1:11">
       <c r="A3414" t="s">
@@ -38368,16 +38361,16 @@
       <c r="B3414">
         <v>117395.02</v>
       </c>
-      <c r="D3414" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3414" s="4"/>
-      <c r="F3414" s="4"/>
-      <c r="G3414" s="4"/>
-      <c r="H3414" s="4"/>
-      <c r="I3414" s="4"/>
-      <c r="J3414" s="4"/>
-      <c r="K3414" s="4"/>
+      <c r="D3414" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3414" s="3"/>
+      <c r="F3414" s="3"/>
+      <c r="G3414" s="3"/>
+      <c r="H3414" s="3"/>
+      <c r="I3414" s="3"/>
+      <c r="J3414" s="3"/>
+      <c r="K3414" s="3"/>
     </row>
     <row r="3415" spans="1:11">
       <c r="A3415" t="s">
@@ -38386,7 +38379,9 @@
       <c r="B3415">
         <v>117395.02</v>
       </c>
-      <c r="D3415" s="4"/>
+      <c r="D3415" s="4" t="s">
+        <v>1</v>
+      </c>
       <c r="E3415" s="4"/>
       <c r="F3415" s="4"/>
       <c r="G3415" s="4"/>
@@ -38395,12 +38390,28 @@
       <c r="J3415" s="4"/>
       <c r="K3415" s="4"/>
     </row>
+    <row r="3416" spans="1:11">
+      <c r="A3416" t="s">
+        <v>3419</v>
+      </c>
+      <c r="B3416">
+        <v>135833.42</v>
+      </c>
+      <c r="D3416" s="4"/>
+      <c r="E3416" s="4"/>
+      <c r="F3416" s="4"/>
+      <c r="G3416" s="4"/>
+      <c r="H3416" s="4"/>
+      <c r="I3416" s="4"/>
+      <c r="J3416" s="4"/>
+      <c r="K3416" s="4"/>
+    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D19:K19"/>
     <mergeCell ref="D20:K21"/>
-    <mergeCell ref="D3413:K3413"/>
-    <mergeCell ref="D3414:K3415"/>
+    <mergeCell ref="D3414:K3414"/>
+    <mergeCell ref="D3415:K3416"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
"Simplificación y Ajuste de Resumen"
</commit_message>
<xml_diff>
--- a/dolartoday.xlsx
+++ b/dolartoday.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3450" uniqueCount="3448">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3458" uniqueCount="3456">
   <si>
     <t>Cotizaciones corresponden al CIERRE del dia</t>
   </si>
@@ -10358,6 +10358,30 @@
   </si>
   <si>
     <t>5-10-2020</t>
+  </si>
+  <si>
+    <t>5-11-2020</t>
+  </si>
+  <si>
+    <t>5-12-2020</t>
+  </si>
+  <si>
+    <t>5-13-2020</t>
+  </si>
+  <si>
+    <t>5-14-2020</t>
+  </si>
+  <si>
+    <t>5-15-2020</t>
+  </si>
+  <si>
+    <t>5-16-2020</t>
+  </si>
+  <si>
+    <t>5-17-2020</t>
+  </si>
+  <si>
+    <t>5-18-2020</t>
   </si>
 </sst>
 </file>
@@ -10494,203 +10518,203 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>DolarToday!$A$3414:$A$3444</c:f>
+              <c:f>DolarToday!$A$3422:$A$3452</c:f>
               <c:strCache>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>4-10-2020</c:v>
+                  <c:v>4-18-2020</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>4-11-2020</c:v>
+                  <c:v>4-19-2020</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4-12-2020</c:v>
+                  <c:v>4-20-2020</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>4-13-2020</c:v>
+                  <c:v>4-21-2020</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4-14-2020</c:v>
+                  <c:v>4-22-2020</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>4-15-2020</c:v>
+                  <c:v>4-23-2020</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4-16-2020</c:v>
+                  <c:v>4-24-2020</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>4-17-2020</c:v>
+                  <c:v>4-25-2020</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4-18-2020</c:v>
+                  <c:v>4-26-2020</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>4-19-2020</c:v>
+                  <c:v>4-27-2020</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>4-20-2020</c:v>
+                  <c:v>4-28-2020</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4-21-2020</c:v>
+                  <c:v>4-29-2020</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>4-22-2020</c:v>
+                  <c:v>4-30-2020</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4-23-2020</c:v>
+                  <c:v>5-1-2020</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>4-24-2020</c:v>
+                  <c:v>5-2-2020</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>4-25-2020</c:v>
+                  <c:v>5-3-2020</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>4-26-2020</c:v>
+                  <c:v>5-4-2020</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>4-27-2020</c:v>
+                  <c:v>5-5-2020</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>4-28-2020</c:v>
+                  <c:v>5-6-2020</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>4-29-2020</c:v>
+                  <c:v>5-7-2020</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>4-30-2020</c:v>
+                  <c:v>5-8-2020</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>5-1-2020</c:v>
+                  <c:v>5-9-2020</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>5-2-2020</c:v>
+                  <c:v>5-10-2020</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5-3-2020</c:v>
+                  <c:v>5-11-2020</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>5-4-2020</c:v>
+                  <c:v>5-12-2020</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>5-5-2020</c:v>
+                  <c:v>5-13-2020</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>5-6-2020</c:v>
+                  <c:v>5-14-2020</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>5-7-2020</c:v>
+                  <c:v>5-15-2020</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5-8-2020</c:v>
+                  <c:v>5-16-2020</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5-9-2020</c:v>
+                  <c:v>5-17-2020</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>5-10-2020</c:v>
+                  <c:v>5-18-2020</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>DolarToday!$B$3414:$B$3444</c:f>
+              <c:f>DolarToday!$B$3422:$B$3452</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>117395.02</c:v>
+                  <c:v>130032.62</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>117395.02</c:v>
+                  <c:v>140102.32</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>135833.42</c:v>
+                  <c:v>153119.32</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>136008.75</c:v>
+                  <c:v>175523.12</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>138053.53</c:v>
+                  <c:v>200058.83</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>134804.72</c:v>
+                  <c:v>195823.41</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>130032.62</c:v>
+                  <c:v>195823.41</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>130032.62</c:v>
+                  <c:v>195823.41</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>130032.62</c:v>
+                  <c:v>197242.02</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>140102.32</c:v>
+                  <c:v>193042.81</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>153119.32</c:v>
+                  <c:v>185004.12</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>175523.12</c:v>
+                  <c:v>180286.55</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>200058.83</c:v>
+                  <c:v>177691.94</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>195823.41</c:v>
+                  <c:v>177691.94</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>195823.41</c:v>
+                  <c:v>177691.94</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>195823.41</c:v>
+                  <c:v>180022.62</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>197242.02</c:v>
+                  <c:v>179021.82</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>193042.81</c:v>
+                  <c:v>175501.44</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>185004.12</c:v>
+                  <c:v>178502.21</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>180286.55</c:v>
+                  <c:v>182042.31</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>177691.94</c:v>
+                  <c:v>182042.31</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>177691.94</c:v>
+                  <c:v>182042.31</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>177691.94</c:v>
+                  <c:v>185201.74</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>180022.62</c:v>
+                  <c:v>182499.03</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>179021.82</c:v>
+                  <c:v>186027.48</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>175501.44</c:v>
+                  <c:v>187704.89</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>178502.21</c:v>
+                  <c:v>188021.12</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>182042.31</c:v>
+                  <c:v>188021.12</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>182042.31</c:v>
+                  <c:v>188021.12</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>182042.31</c:v>
+                  <c:v>187241.82</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>185201.74</c:v>
+                  <c:v>188031.86</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -11097,7 +11121,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:K3444"/>
+  <dimension ref="A1:K3452"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -38669,16 +38693,6 @@
       <c r="B3442">
         <v>182042.31</v>
       </c>
-      <c r="D3442" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3442" s="3"/>
-      <c r="F3442" s="3"/>
-      <c r="G3442" s="3"/>
-      <c r="H3442" s="3"/>
-      <c r="I3442" s="3"/>
-      <c r="J3442" s="3"/>
-      <c r="K3442" s="3"/>
     </row>
     <row r="3443" spans="1:11">
       <c r="A3443" t="s">
@@ -38687,16 +38701,6 @@
       <c r="B3443">
         <v>182042.31</v>
       </c>
-      <c r="D3443" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3443" s="4"/>
-      <c r="F3443" s="4"/>
-      <c r="G3443" s="4"/>
-      <c r="H3443" s="4"/>
-      <c r="I3443" s="4"/>
-      <c r="J3443" s="4"/>
-      <c r="K3443" s="4"/>
     </row>
     <row r="3444" spans="1:11">
       <c r="A3444" t="s">
@@ -38705,21 +38709,105 @@
       <c r="B3444">
         <v>185201.74</v>
       </c>
-      <c r="D3444" s="4"/>
-      <c r="E3444" s="4"/>
-      <c r="F3444" s="4"/>
-      <c r="G3444" s="4"/>
-      <c r="H3444" s="4"/>
-      <c r="I3444" s="4"/>
-      <c r="J3444" s="4"/>
-      <c r="K3444" s="4"/>
+    </row>
+    <row r="3445" spans="1:11">
+      <c r="A3445" t="s">
+        <v>3448</v>
+      </c>
+      <c r="B3445">
+        <v>182499.03</v>
+      </c>
+    </row>
+    <row r="3446" spans="1:11">
+      <c r="A3446" t="s">
+        <v>3449</v>
+      </c>
+      <c r="B3446">
+        <v>186027.48</v>
+      </c>
+    </row>
+    <row r="3447" spans="1:11">
+      <c r="A3447" t="s">
+        <v>3450</v>
+      </c>
+      <c r="B3447">
+        <v>187704.89</v>
+      </c>
+    </row>
+    <row r="3448" spans="1:11">
+      <c r="A3448" t="s">
+        <v>3451</v>
+      </c>
+      <c r="B3448">
+        <v>188021.12</v>
+      </c>
+    </row>
+    <row r="3449" spans="1:11">
+      <c r="A3449" t="s">
+        <v>3452</v>
+      </c>
+      <c r="B3449">
+        <v>188021.12</v>
+      </c>
+    </row>
+    <row r="3450" spans="1:11">
+      <c r="A3450" t="s">
+        <v>3453</v>
+      </c>
+      <c r="B3450">
+        <v>188021.12</v>
+      </c>
+      <c r="D3450" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3450" s="3"/>
+      <c r="F3450" s="3"/>
+      <c r="G3450" s="3"/>
+      <c r="H3450" s="3"/>
+      <c r="I3450" s="3"/>
+      <c r="J3450" s="3"/>
+      <c r="K3450" s="3"/>
+    </row>
+    <row r="3451" spans="1:11">
+      <c r="A3451" t="s">
+        <v>3454</v>
+      </c>
+      <c r="B3451">
+        <v>187241.82</v>
+      </c>
+      <c r="D3451" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3451" s="4"/>
+      <c r="F3451" s="4"/>
+      <c r="G3451" s="4"/>
+      <c r="H3451" s="4"/>
+      <c r="I3451" s="4"/>
+      <c r="J3451" s="4"/>
+      <c r="K3451" s="4"/>
+    </row>
+    <row r="3452" spans="1:11">
+      <c r="A3452" t="s">
+        <v>3455</v>
+      </c>
+      <c r="B3452">
+        <v>188031.86</v>
+      </c>
+      <c r="D3452" s="4"/>
+      <c r="E3452" s="4"/>
+      <c r="F3452" s="4"/>
+      <c r="G3452" s="4"/>
+      <c r="H3452" s="4"/>
+      <c r="I3452" s="4"/>
+      <c r="J3452" s="4"/>
+      <c r="K3452" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="D19:K19"/>
     <mergeCell ref="D20:K21"/>
-    <mergeCell ref="D3442:K3442"/>
-    <mergeCell ref="D3443:K3444"/>
+    <mergeCell ref="D3450:K3450"/>
+    <mergeCell ref="D3451:K3452"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>